<commit_message>
Fix MECH Elective export
</commit_message>
<xml_diff>
--- a/exports/Winter2024_MECH.xlsx
+++ b/exports/Winter2024_MECH.xlsx
@@ -108,8 +108,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="5311573289207638505" xfId="1" hidden="0"/>
-    <cellStyle name="6389168864130269670" xfId="2" hidden="0"/>
+    <cellStyle name="-5574664374842719174" xfId="1" hidden="0"/>
+    <cellStyle name="-8633991114328862649" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>